<commit_message>
layout improvements, asset cleaning, and fixed hardcoded ranking names
</commit_message>
<xml_diff>
--- a/db/dynamic_text.xlsx
+++ b/db/dynamic_text.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10860" yWindow="240" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="15320" yWindow="920" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -160,12 +160,6 @@
     <t>corporate</t>
   </si>
   <si>
-    <t>Intl Gum was incorporated in California on August 2010.</t>
-  </si>
-  <si>
-    <t>The company invested two years in design and development prior to launching the site live near the end of 2012.</t>
-  </si>
-  <si>
     <t>The company headquarters are in San Diego, CA.</t>
   </si>
   <si>
@@ -206,6 +200,12 @@
   </si>
   <si>
     <t>&lt;/br&gt;&lt;/br&gt;&lt;/br&gt;&lt;/br&gt;Members may optionally subscribe to a variety of gum delivered to your door for only $8 per month.</t>
+  </si>
+  <si>
+    <t>The company invested three years in research, design, and development prior to launching live in April 2013.</t>
+  </si>
+  <si>
+    <t>International Gum was incorporated on August 16th 2010 in the Sate of California and does business under the name "Intl Gum".</t>
   </si>
 </sst>
 </file>
@@ -259,7 +259,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="101">
+  <cellStyleXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -334,6 +334,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -370,7 +372,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="101">
+  <cellStyles count="103">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -423,6 +425,7 @@
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -471,6 +474,7 @@
     <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -802,8 +806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView showRuler="0" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -850,7 +854,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -862,12 +866,12 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
@@ -879,7 +883,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1032,7 +1036,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1049,7 +1053,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1117,7 +1121,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1134,7 +1138,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1151,7 +1155,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1474,7 +1478,7 @@
         <v>1</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1508,7 +1512,7 @@
         <v>1</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1525,7 +1529,7 @@
         <v>1</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1542,12 +1546,12 @@
         <v>1</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B44" s="1">
         <v>1</v>
@@ -1559,12 +1563,12 @@
         <v>1</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B45" s="1">
         <v>1</v>
@@ -1576,7 +1580,7 @@
         <v>1</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1594,8 +1598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A48"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection sqref="A1:A45"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A45" sqref="A1:A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1705,13 +1709,13 @@
     <row r="18" spans="1:1">
       <c r="A18" t="str">
         <f>CONCATENATE(Sheet1!A18,"|",Sheet1!B18,"|",Sheet1!C18,"|",Sheet1!D18,"|",Sheet1!E18)</f>
-        <v>corporate|1|14|1|Intl Gum was incorporated in California on August 2010.</v>
+        <v>corporate|1|14|1|International Gum was incorporated on August 16th 2010 in the Sate of California and does business under the name "Intl Gum".</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="str">
         <f>CONCATENATE(Sheet1!A19,"|",Sheet1!B19,"|",Sheet1!C19,"|",Sheet1!D19,"|",Sheet1!E19)</f>
-        <v>corporate|2|14|1|The company invested two years in design and development prior to launching the site live near the end of 2012.</v>
+        <v>corporate|2|14|1|The company invested three years in research, design, and development prior to launching live in April 2013.</v>
       </c>
     </row>
     <row r="20" spans="1:1">

</xml_diff>

<commit_message>
layout fixes and some new assets
</commit_message>
<xml_diff>
--- a/db/dynamic_text.xlsx
+++ b/db/dynamic_text.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15320" yWindow="920" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -196,16 +196,16 @@
     <t>home_slide</t>
   </si>
   <si>
-    <t>&lt;/br&gt;&lt;/br&gt;&lt;/br&gt;&lt;/br&gt;Membership is free and always will be, signup now to rate and vote on gum, along with access to other exclusive offers!</t>
-  </si>
-  <si>
-    <t>&lt;/br&gt;&lt;/br&gt;&lt;/br&gt;&lt;/br&gt;Members may optionally subscribe to a variety of gum delivered to your door for only $8 per month.</t>
-  </si>
-  <si>
     <t>The company invested three years in research, design, and development prior to launching live in April 2013.</t>
   </si>
   <si>
     <t>International Gum was incorporated on August 16th 2010 in the Sate of California and does business under the name "Intl Gum".</t>
+  </si>
+  <si>
+    <t>&lt;/br&gt;&lt;/br&gt;Membership is free and always will be, signup now to rate and vote on gum, along with access to other exclusive offers!</t>
+  </si>
+  <si>
+    <t>&lt;/br&gt;&lt;/br&gt;Members may optionally subscribe to a variety of gum delivered to your door for only $8 per month.</t>
   </si>
 </sst>
 </file>
@@ -259,7 +259,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="103">
+  <cellStyleXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -334,6 +334,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -372,7 +380,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="103">
+  <cellStyles count="111">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -426,6 +434,10 @@
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -475,6 +487,10 @@
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -806,8 +822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -860,13 +876,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -877,13 +893,13 @@
         <v>2</v>
       </c>
       <c r="C4" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1027,7 +1043,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C13" s="1">
         <v>20</v>
@@ -1044,7 +1060,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C14" s="1">
         <v>14</v>
@@ -1121,7 +1137,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1138,7 +1154,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1596,10 +1612,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A48"/>
+  <dimension ref="A1:A52"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A45" sqref="A1:A45"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection sqref="A1:A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1619,13 +1635,13 @@
     <row r="3" spans="1:1">
       <c r="A3" t="str">
         <f>CONCATENATE(Sheet1!A3,"|",Sheet1!B3,"|",Sheet1!C3,"|",Sheet1!D3,"|",Sheet1!E3)</f>
-        <v>home_slide|1|20|1|&lt;/br&gt;&lt;/br&gt;&lt;/br&gt;&lt;/br&gt;Membership is free and always will be, signup now to rate and vote on gum, along with access to other exclusive offers!</v>
+        <v>home_slide|1|30|1|&lt;/br&gt;&lt;/br&gt;Membership is free and always will be, signup now to rate and vote on gum, along with access to other exclusive offers!</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="str">
         <f>CONCATENATE(Sheet1!A4,"|",Sheet1!B4,"|",Sheet1!C4,"|",Sheet1!D4,"|",Sheet1!E4)</f>
-        <v>home_slide|2|20|1|&lt;/br&gt;&lt;/br&gt;&lt;/br&gt;&lt;/br&gt;Members may optionally subscribe to a variety of gum delivered to your door for only $8 per month.</v>
+        <v>home_slide|2|30|1|&lt;/br&gt;&lt;/br&gt;Members may optionally subscribe to a variety of gum delivered to your door for only $8 per month.</v>
       </c>
     </row>
     <row r="5" spans="1:1">
@@ -1679,13 +1695,13 @@
     <row r="13" spans="1:1">
       <c r="A13" t="str">
         <f>CONCATENATE(Sheet1!A13,"|",Sheet1!B13,"|",Sheet1!C13,"|",Sheet1!D13,"|",Sheet1!E13)</f>
-        <v>faq|3|20|1|What type of payment cards do you accept?</v>
+        <v>faq|5|20|1|What type of payment cards do you accept?</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="str">
         <f>CONCATENATE(Sheet1!A14,"|",Sheet1!B14,"|",Sheet1!C14,"|",Sheet1!D14,"|",Sheet1!E14)</f>
-        <v>faq|4|14|1|Intl Gum accepts the following: Visa, MasterCard, American Express, and Discover</v>
+        <v>faq|6|14|1|Intl Gum accepts the following: Visa, MasterCard, American Express, and Discover</v>
       </c>
     </row>
     <row r="15" spans="1:1">
@@ -1889,6 +1905,30 @@
     <row r="48" spans="1:1">
       <c r="A48" t="str">
         <f>CONCATENATE(Sheet1!A48,"|",Sheet1!B48,"|",Sheet1!C48,"|",Sheet1!D48,"|",Sheet1!E48)</f>
+        <v>||||</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="str">
+        <f>CONCATENATE(Sheet1!A49,"|",Sheet1!B49,"|",Sheet1!C49,"|",Sheet1!D49,"|",Sheet1!E49)</f>
+        <v>||||</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="str">
+        <f>CONCATENATE(Sheet1!A50,"|",Sheet1!B50,"|",Sheet1!C50,"|",Sheet1!D50,"|",Sheet1!E50)</f>
+        <v>||||</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="str">
+        <f>CONCATENATE(Sheet1!A51,"|",Sheet1!B51,"|",Sheet1!C51,"|",Sheet1!D51,"|",Sheet1!E51)</f>
+        <v>||||</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="str">
+        <f>CONCATENATE(Sheet1!A52,"|",Sheet1!B52,"|",Sheet1!C52,"|",Sheet1!D52,"|",Sheet1!E52)</f>
         <v>||||</v>
       </c>
     </row>

</xml_diff>

<commit_message>
working on adding support for legal requirements
</commit_message>
<xml_diff>
--- a/db/dynamic_text.xlsx
+++ b/db/dynamic_text.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -259,7 +259,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="113">
+  <cellStyleXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -334,6 +334,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -382,7 +386,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="113">
+  <cellStyles count="117">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -441,6 +445,8 @@
     <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -495,6 +501,8 @@
     <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -826,7 +834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A23" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A27" workbookViewId="0">
       <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
@@ -1618,8 +1626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A52"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection sqref="A1:A45"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
working on recurring billing, and other bug fixes
</commit_message>
<xml_diff>
--- a/db/dynamic_text.xlsx
+++ b/db/dynamic_text.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30060" windowHeight="17420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -202,10 +202,10 @@
     <t>&lt;/br&gt;&lt;/br&gt;Members may optionally subscribe to a variety of gum delivered to your door for only $8 per month.</t>
   </si>
   <si>
-    <t xml:space="preserve">Note: Intl Gum holds no liability for the accuracy of the above information, description, ingredients, etc. Always consult information on the product packaging before consumption. All gum names, images, designs, brands, and Trademarks are property of the product owner (not Intl Gum). No image may not be used without the express permission of the company and product owner.  </t>
-  </si>
-  <si>
-    <t>All gum names, images, designs, brands, and Trademarks are property of the product owners (not Intl Gum). No images may be used without the express permission of each respective company and product owner.</t>
+    <t>Please Note: All ratings/comments were created by Intl Gum members, neither Intl Gum nor the product owner hold any liability for these ratings/comments, and furthermore these ratings/comments are not the views of Intl Gum nor the product owners.  All gum names, images, designs, brands, and Trademarks are property of the product owners (not Intl Gum). No images or names may be used without the express permission of each respective company and product owner.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please Note: All ratings/comments were created by Intl Gum members, neither Intl Gum nor the product owner hold any liability for these ratings/comments, and furthermore these ratings/comments are not the views of Intl Gum nor the product owners.  Intl Gum also holds no liability for the accuracy of the above information, description, ingredients, etc. Always consult information on the product packaging before consumption. All gum names, images, designs, brands, and Trademarks are property of the product owner (not Intl Gum). No image or name may not be used without the express permission of the company and product owner.  </t>
   </si>
 </sst>
 </file>
@@ -835,7 +835,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1591,7 +1591,7 @@
         <v>1</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1608,7 +1608,7 @@
         <v>1</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1893,13 +1893,13 @@
     <row r="44" spans="1:1">
       <c r="A44" t="str">
         <f>CONCATENATE(Sheet1!A44,"|",Sheet1!B44,"|",Sheet1!C44,"|",Sheet1!D44,"|",Sheet1!E44)</f>
-        <v xml:space="preserve">gum_specific|1|8|1|Note: Intl Gum holds no liability for the accuracy of the above information, description, ingredients, etc. Always consult information on the product packaging before consumption. All gum names, images, designs, brands, and Trademarks are property of the product owner (not Intl Gum). No image may not be used without the express permission of the company and product owner.  </v>
+        <v xml:space="preserve">gum_specific|1|8|1|Please Note: All ratings/comments were created by Intl Gum members, neither Intl Gum nor the product owner hold any liability for these ratings/comments, and furthermore these ratings/comments are not the views of Intl Gum nor the product owners.  Intl Gum also holds no liability for the accuracy of the above information, description, ingredients, etc. Always consult information on the product packaging before consumption. All gum names, images, designs, brands, and Trademarks are property of the product owner (not Intl Gum). No image or name may not be used without the express permission of the company and product owner.  </v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="str">
         <f>CONCATENATE(Sheet1!A45,"|",Sheet1!B45,"|",Sheet1!C45,"|",Sheet1!D45,"|",Sheet1!E45)</f>
-        <v>gum_general|1|8|1|All gum names, images, designs, brands, and Trademarks are property of the product owners (not Intl Gum). No images may be used without the express permission of each respective company and product owner.</v>
+        <v>gum_general|1|8|1|Please Note: All ratings/comments were created by Intl Gum members, neither Intl Gum nor the product owner hold any liability for these ratings/comments, and furthermore these ratings/comments are not the views of Intl Gum nor the product owners.  All gum names, images, designs, brands, and Trademarks are property of the product owners (not Intl Gum). No images or names may be used without the express permission of each respective company and product owner.</v>
       </c>
     </row>
     <row r="46" spans="1:1">

</xml_diff>

<commit_message>
clean up side bar options and all linkage/naming
</commit_message>
<xml_diff>
--- a/db/dynamic_text.xlsx
+++ b/db/dynamic_text.xlsx
@@ -97,9 +97,6 @@
     <t>Intl Gum Members also have the option of paying for a monthly subscription, which delivers a variety of gum directly to your door every month via mail.  On average you will receive a half dozen different packs of gum, about 100 pieces of gum total.</t>
   </si>
   <si>
-    <t>Monthly subscriptions are always only $8 per month, automatically billed on the 8th day of every month.  You may cancel your recurring subscription at any time via your account info page (same place you sign up) or by contacting Intl Gum customer support directly.</t>
-  </si>
-  <si>
     <t>All content from your optional Private information section (clearly displayed area within Your Account page) is always kept in absolute private and never displayed publicly.  This information includes mailing address, billing name, and billing info.  Your payment information is never stored in our system (if entered for the optional monthly Subscription plan).  We ask for your name, address and contact information so we can send you your monthly gum. We ask for credit card information so we can fulfill your subscription, and so we can provide this information to the company or companies who process your credit card payment. We do not share any other information with third parties.</t>
   </si>
   <si>
@@ -190,12 +187,6 @@
     <t>home_slide</t>
   </si>
   <si>
-    <t>The company invested three years in research, design, and development prior to launching live in April 2013.</t>
-  </si>
-  <si>
-    <t>International Gum was incorporated on August 16th 2010 in the Sate of California and does business under the name "Intl Gum".</t>
-  </si>
-  <si>
     <t>&lt;/br&gt;&lt;/br&gt;Membership is free and always will be, signup now to rate and vote on gum, along with access to other exclusive offers!</t>
   </si>
   <si>
@@ -206,6 +197,15 @@
   </si>
   <si>
     <t xml:space="preserve">Please Note: All ratings/comments were created by Intl Gum members, neither Intl Gum nor the product owner hold any liability for these ratings/comments, and furthermore these ratings/comments are not the views of Intl Gum nor the product owners.  Intl Gum also holds no liability for the accuracy of the above information, description, ingredients, etc. Always consult information on the product packaging before consumption. All gum names, images, designs, brands, and Trademarks are property of the product owner (not Intl Gum). No image or name may not be used without the express permission of the company and product owner.  </t>
+  </si>
+  <si>
+    <t>Monthly subscriptions are always only $8 per month, automatically billed on the 8th day of every month.  You may cancel your recurring subscription at any time via your account info page (same place you sign up) or by contacting Intl Gum customer support directly.  There are no additional costs for shipping and handling.</t>
+  </si>
+  <si>
+    <t>International Gum is a small start up company that was founded by Kevin Andrew Hoiland and incorporated on August 16th 2010 in the Sate of California.  International Gum Inc also does business under the name "Intl Gum".</t>
+  </si>
+  <si>
+    <t>The company invested three years in research, design, and development prior to launching this website live in April 2013.</t>
   </si>
 </sst>
 </file>
@@ -239,7 +239,8 @@
     <font>
       <sz val="12"/>
       <color rgb="FF323537"/>
-      <name val="Helvetica"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -834,21 +835,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.5" style="1" customWidth="1"/>
     <col min="2" max="4" width="10.83203125" style="1"/>
-    <col min="5" max="5" width="19.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="146" style="1" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1">
         <v>1</v>
@@ -860,12 +861,12 @@
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -877,12 +878,12 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -894,12 +895,12 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
@@ -911,7 +912,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1064,7 +1065,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1081,7 +1082,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1132,12 +1133,12 @@
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
@@ -1149,12 +1150,12 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B19" s="1">
         <v>2</v>
@@ -1166,12 +1167,12 @@
         <v>1</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="1">
         <v>3</v>
@@ -1183,7 +1184,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1234,7 +1235,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1302,7 +1303,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1319,7 +1320,7 @@
         <v>1</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1370,7 +1371,7 @@
         <v>1</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1392,7 +1393,7 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B33" s="1">
         <v>1</v>
@@ -1404,12 +1405,12 @@
         <v>1</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B34" s="1">
         <v>1</v>
@@ -1420,13 +1421,13 @@
       <c r="D34" s="1">
         <v>1</v>
       </c>
-      <c r="E34" t="s">
-        <v>28</v>
+      <c r="E34" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B35" s="1">
         <v>2</v>
@@ -1437,13 +1438,13 @@
       <c r="D35" s="1">
         <v>1</v>
       </c>
-      <c r="E35" t="s">
-        <v>31</v>
+      <c r="E35" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="1">
         <v>1</v>
@@ -1455,12 +1456,12 @@
         <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" s="1">
         <v>2</v>
@@ -1472,12 +1473,12 @@
         <v>1</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B38" s="1">
         <v>1</v>
@@ -1489,12 +1490,12 @@
         <v>1</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B39" s="1">
         <v>2</v>
@@ -1506,12 +1507,12 @@
         <v>1</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B40" s="1">
         <v>3</v>
@@ -1523,12 +1524,12 @@
         <v>1</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41" s="1">
         <v>4</v>
@@ -1540,12 +1541,12 @@
         <v>1</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42" s="1">
         <v>5</v>
@@ -1557,12 +1558,12 @@
         <v>1</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" s="1">
         <v>6</v>
@@ -1574,12 +1575,12 @@
         <v>1</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B44" s="1">
         <v>1</v>
@@ -1591,12 +1592,12 @@
         <v>1</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B45" s="1">
         <v>1</v>
@@ -1608,7 +1609,7 @@
         <v>1</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1731,19 +1732,19 @@
     <row r="17" spans="1:1">
       <c r="A17" t="str">
         <f>CONCATENATE(Sheet1!A17,"|",Sheet1!B17,"|",Sheet1!C17,"|",Sheet1!D17,"|",Sheet1!E17)</f>
-        <v>about|3|16|1|Monthly subscriptions are always only $8 per month, automatically billed on the 8th day of every month.  You may cancel your recurring subscription at any time via your account info page (same place you sign up) or by contacting Intl Gum customer support directly.</v>
+        <v>about|3|16|1|Monthly subscriptions are always only $8 per month, automatically billed on the 8th day of every month.  You may cancel your recurring subscription at any time via your account info page (same place you sign up) or by contacting Intl Gum customer support directly.  There are no additional costs for shipping and handling.</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="str">
         <f>CONCATENATE(Sheet1!A18,"|",Sheet1!B18,"|",Sheet1!C18,"|",Sheet1!D18,"|",Sheet1!E18)</f>
-        <v>corporate|1|14|1|International Gum was incorporated on August 16th 2010 in the Sate of California and does business under the name "Intl Gum".</v>
+        <v>corporate|1|14|1|International Gum is a small start up company that was founded by Kevin Andrew Hoiland and incorporated on August 16th 2010 in the Sate of California.  International Gum Inc also does business under the name "Intl Gum".</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="str">
         <f>CONCATENATE(Sheet1!A19,"|",Sheet1!B19,"|",Sheet1!C19,"|",Sheet1!D19,"|",Sheet1!E19)</f>
-        <v>corporate|2|14|1|The company invested three years in research, design, and development prior to launching live in April 2013.</v>
+        <v>corporate|2|14|1|The company invested three years in research, design, and development prior to launching this website live in April 2013.</v>
       </c>
     </row>
     <row r="20" spans="1:1">

</xml_diff>

<commit_message>
fuck yeah!  gums show pages basically done and look bomb :-)
</commit_message>
<xml_diff>
--- a/db/dynamic_text.xlsx
+++ b/db/dynamic_text.xlsx
@@ -190,9 +190,6 @@
     <t>&lt;/br&gt;&lt;/br&gt;Membership is free and always will be, signup now to rate and vote on gum, along with access to other exclusive offers!</t>
   </si>
   <si>
-    <t>&lt;/br&gt;&lt;/br&gt;Members may optionally subscribe to a variety of gum delivered to your door for only $8 per month.</t>
-  </si>
-  <si>
     <t>Please Note: All ratings/comments were created by Intl Gum members, neither Intl Gum nor the product owner hold any liability for these ratings/comments, and furthermore these ratings/comments are not the views of Intl Gum nor the product owners.  All gum names, images, designs, brands, and Trademarks are property of the product owners (not Intl Gum). No images or names may be used without the express permission of each respective company and product owner.</t>
   </si>
   <si>
@@ -206,6 +203,9 @@
   </si>
   <si>
     <t>The company invested three years in research, design, and development prior to launching this website live in April 2013.</t>
+  </si>
+  <si>
+    <t>&lt;/br&gt;&lt;/br&gt;Members may optionally subscribe to a variety of gum delivered to their door for only $8 per month.</t>
   </si>
 </sst>
 </file>
@@ -836,7 +836,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -912,7 +912,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1133,7 +1133,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1150,7 +1150,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1167,7 +1167,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1592,7 +1592,7 @@
         <v>1</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1609,7 +1609,7 @@
         <v>1</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1654,7 +1654,7 @@
     <row r="4" spans="1:1">
       <c r="A4" t="str">
         <f>CONCATENATE(Sheet1!A4,"|",Sheet1!B4,"|",Sheet1!C4,"|",Sheet1!D4,"|",Sheet1!E4)</f>
-        <v>home_slide|2|30|1|&lt;/br&gt;&lt;/br&gt;Members may optionally subscribe to a variety of gum delivered to your door for only $8 per month.</v>
+        <v>home_slide|2|30|1|&lt;/br&gt;&lt;/br&gt;Members may optionally subscribe to a variety of gum delivered to their door for only $8 per month.</v>
       </c>
     </row>
     <row r="5" spans="1:1">

</xml_diff>

<commit_message>
finished mailers and created ratings show page
</commit_message>
<xml_diff>
--- a/db/dynamic_text.xlsx
+++ b/db/dynamic_text.xlsx
@@ -187,9 +187,6 @@
     <t>Please Note: All ratings/comments were created by Intl Gum members, neither Intl Gum nor the product owner hold any liability for these ratings/comments, and furthermore these ratings/comments are not the views of Intl Gum nor the product owners.  All gum names, images, designs, brands, and Trademarks are property of the product owners (not Intl Gum). No images or names may be used without the express permission of each respective company and product owner.</t>
   </si>
   <si>
-    <t xml:space="preserve">Please Note: All ratings/comments were created by Intl Gum members, neither Intl Gum nor the product owner hold any liability for these ratings/comments, and furthermore these ratings/comments are not the views of Intl Gum nor the product owners.  Intl Gum also holds no liability for the accuracy of the above information, description, ingredients, etc. Always consult information on the product packaging before consumption. All gum names, images, designs, brands, and Trademarks are property of the product owner (not Intl Gum). No image or name may not be used without the express permission of the company and product owner.  </t>
-  </si>
-  <si>
     <t>Monthly subscriptions are always only $8 per month, automatically billed on the 8th day of every month.  You may cancel your recurring subscription at any time via your account info page (same place you sign up) or by contacting Intl Gum customer support directly.  There are no additional costs for shipping and handling.</t>
   </si>
   <si>
@@ -206,6 +203,9 @@
   </si>
   <si>
     <t>Intl Gum Membership is free, which allows you to vote, rank, and comment on Gums. The Intl Gum Subscription offer, however, is an optional service that costs $8 per month, automatically charging your credit card on the 8th day of every month. There is no long term commitment and you may choose to subscribe or unsubscribe at any time. An Intl Gum Subscription provides you with a variety of Gum delivered directly to your door every month.  There is no additional cost for shipping and handling.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please Note: All ratings/comments were created by Intl Gum members, neither Intl Gum nor the product owner hold any liability for these ratings/comments, and furthermore these ratings/comments are not necessarily the views of Intl Gum nor the product owners.  Intl Gum also holds no liability for the accuracy of the above information, description, ingredients, etc. Always consult information on the product packaging before consumption. All gum names, images, designs, brands, and Trademarks are property of the product owner (not Intl Gum). No image or name may not be used without the express permission of the company and product owner.  </t>
   </si>
 </sst>
 </file>
@@ -839,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -916,7 +916,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1137,7 +1137,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1154,7 +1154,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1171,7 +1171,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1409,7 +1409,7 @@
         <v>1</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1426,7 +1426,7 @@
         <v>1</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1596,7 +1596,7 @@
         <v>1</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1898,7 +1898,7 @@
     <row r="44" spans="1:1">
       <c r="A44" t="str">
         <f>CONCATENATE(Sheet1!A44,"|",Sheet1!B44,"|",Sheet1!C44,"|",Sheet1!D44,"|",Sheet1!E44)</f>
-        <v xml:space="preserve">gum_specific|1|8|1|Please Note: All ratings/comments were created by Intl Gum members, neither Intl Gum nor the product owner hold any liability for these ratings/comments, and furthermore these ratings/comments are not the views of Intl Gum nor the product owners.  Intl Gum also holds no liability for the accuracy of the above information, description, ingredients, etc. Always consult information on the product packaging before consumption. All gum names, images, designs, brands, and Trademarks are property of the product owner (not Intl Gum). No image or name may not be used without the express permission of the company and product owner.  </v>
+        <v xml:space="preserve">gum_specific|1|8|1|Please Note: All ratings/comments were created by Intl Gum members, neither Intl Gum nor the product owner hold any liability for these ratings/comments, and furthermore these ratings/comments are not necessarily the views of Intl Gum nor the product owners.  Intl Gum also holds no liability for the accuracy of the above information, description, ingredients, etc. Always consult information on the product packaging before consumption. All gum names, images, designs, brands, and Trademarks are property of the product owner (not Intl Gum). No image or name may not be used without the express permission of the company and product owner.  </v>
       </c>
     </row>
     <row r="45" spans="1:1">

</xml_diff>

<commit_message>
implemented de-active gum in View, added image TMs, & more seed data
</commit_message>
<xml_diff>
--- a/db/dynamic_text.xlsx
+++ b/db/dynamic_text.xlsx
@@ -67,9 +67,6 @@
     <t>Please contact Intl Gum at any time!  The phone number is toll free and thus no cost to you.</t>
   </si>
   <si>
-    <t>We are also available via email if desired.</t>
-  </si>
-  <si>
     <t>You may cancel your ongoing subscription membership at any time on your Membership Account Info page or by contacting Intl Gum customer support. All cancellation requests must be received before the billing cycle of the next upcoming month (always the 8th calendar day of each month). Cancellation requests received after the eight day of a month shall apply to the following month.</t>
   </si>
   <si>
@@ -206,6 +203,9 @@
   </si>
   <si>
     <t xml:space="preserve">Please Note: All ratings/comments were created by Intl Gum members, neither Intl Gum nor the product owner hold any liability for these ratings/comments, and furthermore these ratings/comments are not necessarily the views of Intl Gum nor the product owners.  Intl Gum also holds no liability for the accuracy of the above information, description, ingredients, etc. Always consult information on the product packaging before consumption. All gum names, images, designs, brands, and Trademarks are property of the product owner (not Intl Gum). No image or name may not be used without the express permission of the company and product owner.  </t>
+  </si>
+  <si>
+    <t>We are also available via email and social media.</t>
   </si>
 </sst>
 </file>
@@ -839,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -853,7 +853,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1">
         <v>1</v>
@@ -865,12 +865,12 @@
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -882,12 +882,12 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -899,12 +899,12 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
@@ -916,7 +916,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -967,7 +967,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1069,7 +1069,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1086,7 +1086,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1103,7 +1103,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1120,7 +1120,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1137,12 +1137,12 @@
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
@@ -1154,12 +1154,12 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="1">
         <v>2</v>
@@ -1171,12 +1171,12 @@
         <v>1</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="1">
         <v>3</v>
@@ -1188,7 +1188,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1239,7 +1239,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1256,7 +1256,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1273,12 +1273,12 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B26" s="1">
         <v>1</v>
@@ -1290,12 +1290,12 @@
         <v>1</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B27" s="1">
         <v>2</v>
@@ -1307,12 +1307,12 @@
         <v>1</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B28" s="1">
         <v>3</v>
@@ -1324,12 +1324,12 @@
         <v>1</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B29" s="1">
         <v>4</v>
@@ -1341,12 +1341,12 @@
         <v>1</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B30" s="1">
         <v>5</v>
@@ -1358,12 +1358,12 @@
         <v>1</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B31" s="1">
         <v>6</v>
@@ -1375,12 +1375,12 @@
         <v>1</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B32" s="1">
         <v>7</v>
@@ -1392,12 +1392,12 @@
         <v>1</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B33" s="1">
         <v>1</v>
@@ -1409,12 +1409,12 @@
         <v>1</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B34" s="1">
         <v>1</v>
@@ -1426,12 +1426,12 @@
         <v>1</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B35" s="1">
         <v>2</v>
@@ -1443,12 +1443,12 @@
         <v>1</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B36" s="1">
         <v>1</v>
@@ -1460,12 +1460,12 @@
         <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B37" s="1">
         <v>2</v>
@@ -1477,12 +1477,12 @@
         <v>1</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38" s="1">
         <v>1</v>
@@ -1494,12 +1494,12 @@
         <v>1</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" s="1">
         <v>2</v>
@@ -1511,12 +1511,12 @@
         <v>1</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" s="1">
         <v>3</v>
@@ -1528,12 +1528,12 @@
         <v>1</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" s="1">
         <v>4</v>
@@ -1545,12 +1545,12 @@
         <v>1</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B42" s="1">
         <v>5</v>
@@ -1562,12 +1562,12 @@
         <v>1</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B43" s="1">
         <v>6</v>
@@ -1579,12 +1579,12 @@
         <v>1</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B44" s="1">
         <v>1</v>
@@ -1596,12 +1596,12 @@
         <v>1</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B45" s="1">
         <v>1</v>
@@ -1613,7 +1613,7 @@
         <v>1</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1676,7 +1676,7 @@
     <row r="7" spans="1:1">
       <c r="A7" t="str">
         <f>CONCATENATE(Sheet1!A7,"|",Sheet1!B7,"|",Sheet1!C7,"|",Sheet1!D7,"|",Sheet1!E7)</f>
-        <v>contact|3|14|1|We are also available via email if desired.</v>
+        <v>contact|3|14|1|We are also available via email and social media.</v>
       </c>
     </row>
     <row r="8" spans="1:1">

</xml_diff>